<commit_message>
[IMP] 添加0.19.0 changelog;修改 README.md;调整菜单顺序;删除移除saga和sagaTask的job
</commit_message>
<xml_diff>
--- a/src/main/resources/script/meta/micro-service-init-data.xlsx
+++ b/src/main/resources/script/meta/micro-service-init-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540" tabRatio="500" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="12540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IAM_PERMISSION" sheetId="1" r:id="rId1"/>
@@ -403,10 +403,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -456,15 +456,17 @@
       <charset val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -486,7 +488,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -501,7 +563,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -515,14 +592,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -532,81 +601,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Arial"/>
       <charset val="1"/>
@@ -621,187 +621,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -812,15 +812,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -856,6 +847,39 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -880,30 +904,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -915,148 +915,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1620,8 +1620,8 @@
   <sheetPr/>
   <dimension ref="D7:P14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1713,7 +1713,7 @@
         <v>44</v>
       </c>
       <c r="O8" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="6:15">
@@ -1745,7 +1745,7 @@
         <v>48</v>
       </c>
       <c r="O9" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="6:15">
@@ -1775,7 +1775,7 @@
         <v>53</v>
       </c>
       <c r="O10" s="4">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="6:15">
@@ -1871,7 +1871,7 @@
         <v>48</v>
       </c>
       <c r="O13" s="4">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="6:15">
@@ -2269,7 +2269,7 @@
   <sheetPr/>
   <dimension ref="D7:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>

</xml_diff>